<commit_message>
Started working on multithreaded mergesort
</commit_message>
<xml_diff>
--- a/submit/results formatted.xlsx
+++ b/submit/results formatted.xlsx
@@ -1,36 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ethan\Documents\GitHub\CSC382-Algorithms-Labs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan\Documents\GitHub\CSC382-Algorithms-Labs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175DDC07-BB34-4B84-84B8-1053F90E3052}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB32E280-1E9D-4D1D-A107-D37535AEBD12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results formatted" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
-  <si>
-    <t>INSERTION SORT</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="13">
   <si>
     <t>BOUNDS</t>
   </si>
@@ -47,16 +37,28 @@
     <t>RAND</t>
   </si>
   <si>
-    <t>MERGE SORT</t>
-  </si>
-  <si>
     <t>Blue = Insertion</t>
   </si>
   <si>
     <t>Green = Merge</t>
   </si>
   <si>
-    <t>BEST RESULTS</t>
+    <t>BEST RESULTS: TIME</t>
+  </si>
+  <si>
+    <t>INSERTION SORT: TIME</t>
+  </si>
+  <si>
+    <t>MERGE SORT: TIME</t>
+  </si>
+  <si>
+    <t>MERGE SORT: STEPS</t>
+  </si>
+  <si>
+    <t>INSERTION SORT: STEPS</t>
+  </si>
+  <si>
+    <t>BEST RESULTS: STEPS</t>
   </si>
 </sst>
 </file>
@@ -380,7 +382,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -495,6 +497,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -540,7 +583,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2"/>
@@ -548,6 +591,10 @@
     <xf numFmtId="0" fontId="17" fillId="29" borderId="5" xfId="38" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="25" borderId="0" xfId="34"/>
     <xf numFmtId="0" fontId="17" fillId="29" borderId="0" xfId="38"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="11" xfId="9" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="12" xfId="9" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="10" xfId="34" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="10" xfId="38" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3439,25 +3486,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:S31"/>
+  <dimension ref="A2:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26:N31"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S41" sqref="S41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1">
         <v>100</v>
@@ -3484,7 +3535,7 @@
         <v>10000</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" s="1">
         <v>100</v>
@@ -3513,7 +3564,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="3">
         <v>2013</v>
@@ -3540,7 +3591,7 @@
         <v>15603</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L4" s="4">
         <v>14833</v>
@@ -3569,7 +3620,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="3">
         <v>51229</v>
@@ -3596,7 +3647,7 @@
         <v>18719039</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L5" s="4">
         <v>5544</v>
@@ -3625,7 +3676,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="3">
         <v>6958</v>
@@ -3652,7 +3703,7 @@
         <v>8698761</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L6" s="4">
         <v>7953</v>
@@ -3681,7 +3732,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="3">
         <v>1687</v>
@@ -3708,7 +3759,7 @@
         <v>8663365</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L7" s="4">
         <v>8045</v>
@@ -3735,194 +3786,660 @@
         <v>927490</v>
       </c>
     </row>
-    <row r="26" spans="6:14" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F26" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J26" s="5" t="s">
+    <row r="25" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="8">
+        <v>100</v>
+      </c>
+      <c r="C26" s="8">
+        <v>200</v>
+      </c>
+      <c r="D26" s="8">
+        <v>300</v>
+      </c>
+      <c r="E26" s="8">
+        <v>400</v>
+      </c>
+      <c r="F26" s="8">
+        <v>500</v>
+      </c>
+      <c r="G26" s="8">
+        <v>1000</v>
+      </c>
+      <c r="H26" s="8">
+        <v>4000</v>
+      </c>
+      <c r="I26" s="8">
+        <v>10000</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L26" s="8">
+        <v>100</v>
+      </c>
+      <c r="M26" s="8">
+        <v>200</v>
+      </c>
+      <c r="N26" s="8">
+        <v>300</v>
+      </c>
+      <c r="O26" s="8">
+        <v>400</v>
+      </c>
+      <c r="P26" s="8">
+        <v>500</v>
+      </c>
+      <c r="Q26" s="8">
+        <v>1000</v>
+      </c>
+      <c r="R26" s="8">
+        <v>4000</v>
+      </c>
+      <c r="S26" s="8">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="9">
+        <v>794</v>
+      </c>
+      <c r="C27" s="9">
+        <v>1594</v>
+      </c>
+      <c r="D27" s="9">
+        <v>2394</v>
+      </c>
+      <c r="E27" s="9">
+        <v>3194</v>
+      </c>
+      <c r="F27" s="9">
+        <v>3994</v>
+      </c>
+      <c r="G27" s="9">
+        <v>7994</v>
+      </c>
+      <c r="H27" s="9">
+        <v>31994</v>
+      </c>
+      <c r="I27" s="9">
+        <v>79994</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L27" s="10">
+        <v>6428</v>
+      </c>
+      <c r="M27" s="10">
+        <v>14272</v>
+      </c>
+      <c r="N27" s="10">
+        <v>22628</v>
+      </c>
+      <c r="O27" s="10">
+        <v>31360</v>
+      </c>
+      <c r="P27" s="10">
+        <v>39956</v>
+      </c>
+      <c r="Q27" s="10">
+        <v>86928</v>
+      </c>
+      <c r="R27" s="10">
+        <v>403760</v>
+      </c>
+      <c r="S27" s="10">
+        <v>1109696</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="9">
+        <v>15644</v>
+      </c>
+      <c r="C28" s="9">
+        <v>61294</v>
+      </c>
+      <c r="D28" s="9">
+        <v>136944</v>
+      </c>
+      <c r="E28" s="9">
+        <v>242594</v>
+      </c>
+      <c r="F28" s="9">
+        <v>378244</v>
+      </c>
+      <c r="G28" s="9">
+        <v>1506494</v>
+      </c>
+      <c r="H28" s="9">
+        <v>24025994</v>
+      </c>
+      <c r="I28" s="9">
+        <v>150064994</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L28" s="10">
+        <v>6447</v>
+      </c>
+      <c r="M28" s="10">
+        <v>14311</v>
+      </c>
+      <c r="N28" s="10">
+        <v>22671</v>
+      </c>
+      <c r="O28" s="10">
+        <v>31439</v>
+      </c>
+      <c r="P28" s="10">
+        <v>40343</v>
+      </c>
+      <c r="Q28" s="10">
+        <v>87703</v>
+      </c>
+      <c r="R28" s="10">
+        <v>406863</v>
+      </c>
+      <c r="S28" s="10">
+        <v>1110895</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="9">
+        <v>8293</v>
+      </c>
+      <c r="C29" s="9">
+        <v>30995</v>
+      </c>
+      <c r="D29" s="9">
+        <v>69217</v>
+      </c>
+      <c r="E29" s="9">
+        <v>122660</v>
+      </c>
+      <c r="F29" s="9">
+        <v>191240</v>
+      </c>
+      <c r="G29" s="9">
+        <v>758426</v>
+      </c>
+      <c r="H29" s="9">
+        <v>12015722</v>
+      </c>
+      <c r="I29" s="9">
+        <v>75139012</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L29" s="10">
+        <v>6852</v>
+      </c>
+      <c r="M29" s="10">
+        <v>15321</v>
+      </c>
+      <c r="N29" s="10">
+        <v>24372</v>
+      </c>
+      <c r="O29" s="10">
+        <v>33860</v>
+      </c>
+      <c r="P29" s="10">
+        <v>43378</v>
+      </c>
+      <c r="Q29" s="10">
+        <v>94759</v>
+      </c>
+      <c r="R29" s="10">
+        <v>443086</v>
+      </c>
+      <c r="S29" s="10">
+        <v>1218069</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="9">
+        <v>8098</v>
+      </c>
+      <c r="C30" s="9">
+        <v>31270</v>
+      </c>
+      <c r="D30" s="9">
+        <v>69316</v>
+      </c>
+      <c r="E30" s="9">
+        <v>122905</v>
+      </c>
+      <c r="F30" s="9">
+        <v>189446</v>
+      </c>
+      <c r="G30" s="9">
+        <v>755635</v>
+      </c>
+      <c r="H30" s="9">
+        <v>12022168</v>
+      </c>
+      <c r="I30" s="9">
+        <v>75030572</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L30" s="10">
+        <v>6853</v>
+      </c>
+      <c r="M30" s="10">
+        <v>15320</v>
+      </c>
+      <c r="N30" s="10">
+        <v>24370</v>
+      </c>
+      <c r="O30" s="10">
+        <v>33856</v>
+      </c>
+      <c r="P30" s="10">
+        <v>43365</v>
+      </c>
+      <c r="Q30" s="10">
+        <v>94764</v>
+      </c>
+      <c r="R30" s="10">
+        <v>443075</v>
+      </c>
+      <c r="S30" s="10">
+        <v>1218092</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K26" s="5"/>
-      <c r="M26" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="N26" s="6"/>
+      <c r="E33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" s="5"/>
+      <c r="H33" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I33" s="6"/>
+      <c r="K33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P33" s="5"/>
+      <c r="R33" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="S33" s="6"/>
     </row>
-    <row r="27" spans="6:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="F27" s="1" t="s">
+    <row r="34" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="1">
+        <v>100</v>
+      </c>
+      <c r="C34" s="1">
+        <v>200</v>
+      </c>
+      <c r="D34" s="1">
+        <v>300</v>
+      </c>
+      <c r="E34" s="1">
+        <v>400</v>
+      </c>
+      <c r="F34" s="1">
+        <v>500</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H34" s="1">
+        <v>4000</v>
+      </c>
+      <c r="I34" s="1">
+        <v>10000</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L34" s="1">
+        <v>100</v>
+      </c>
+      <c r="M34" s="1">
+        <v>200</v>
+      </c>
+      <c r="N34" s="1">
+        <v>300</v>
+      </c>
+      <c r="O34" s="1">
+        <v>400</v>
+      </c>
+      <c r="P34" s="1">
+        <v>500</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>1000</v>
+      </c>
+      <c r="R34" s="1">
+        <v>4000</v>
+      </c>
+      <c r="S34" s="1">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G27" s="1">
-        <v>100</v>
-      </c>
-      <c r="H27" s="1">
-        <v>200</v>
-      </c>
-      <c r="I27" s="1">
-        <v>300</v>
-      </c>
-      <c r="J27" s="1">
-        <v>400</v>
-      </c>
-      <c r="K27" s="1">
-        <v>500</v>
-      </c>
-      <c r="L27" s="1">
-        <v>1000</v>
-      </c>
-      <c r="M27" s="1">
-        <v>4000</v>
-      </c>
-      <c r="N27" s="1">
+      <c r="B35" s="5">
+        <f>MIN(B4, L4)</f>
+        <v>2013</v>
+      </c>
+      <c r="C35" s="5">
+        <f>MIN(C4, M4)</f>
+        <v>360</v>
+      </c>
+      <c r="D35" s="5">
+        <f>MIN(D4, N4)</f>
+        <v>458</v>
+      </c>
+      <c r="E35" s="5">
+        <f>MIN(E4, O4)</f>
+        <v>614</v>
+      </c>
+      <c r="F35" s="5">
+        <f>MIN(F4, P4)</f>
+        <v>731</v>
+      </c>
+      <c r="G35" s="5">
+        <f>MIN(G4, Q4)</f>
+        <v>1409</v>
+      </c>
+      <c r="H35" s="5">
+        <f>MIN(H4, R4)</f>
+        <v>5563</v>
+      </c>
+      <c r="I35" s="5">
+        <f>MIN(I4, S4)</f>
+        <v>15603</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L35" s="5">
+        <f>MIN(B27, L27)</f>
+        <v>794</v>
+      </c>
+      <c r="M35" s="5">
+        <f t="shared" ref="M35:S35" si="0">MIN(C27, M27)</f>
+        <v>1594</v>
+      </c>
+      <c r="N35" s="5">
+        <f t="shared" si="0"/>
+        <v>2394</v>
+      </c>
+      <c r="O35" s="5">
+        <f t="shared" si="0"/>
+        <v>3194</v>
+      </c>
+      <c r="P35" s="5">
+        <f t="shared" si="0"/>
+        <v>3994</v>
+      </c>
+      <c r="Q35" s="5">
+        <f t="shared" si="0"/>
+        <v>7994</v>
+      </c>
+      <c r="R35" s="5">
+        <f t="shared" si="0"/>
+        <v>31994</v>
+      </c>
+      <c r="S35" s="5">
+        <f t="shared" si="0"/>
+        <v>79994</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="6">
+        <f>MIN(B5, L5)</f>
+        <v>5544</v>
+      </c>
+      <c r="C36" s="5">
+        <f>MIN(C5, M5)</f>
+        <v>7631</v>
+      </c>
+      <c r="D36" s="5">
+        <f>MIN(D5, N5)</f>
+        <v>16964</v>
+      </c>
+      <c r="E36" s="6">
+        <f>MIN(E5, O5)</f>
+        <v>23254</v>
+      </c>
+      <c r="F36" s="6">
+        <f>MIN(F5, P5)</f>
+        <v>29939</v>
+      </c>
+      <c r="G36" s="6">
+        <f>MIN(G5, Q5)</f>
+        <v>76049</v>
+      </c>
+      <c r="H36" s="6">
+        <f>MIN(H5, R5)</f>
+        <v>147002</v>
+      </c>
+      <c r="I36" s="6">
+        <f>MIN(I5, S5)</f>
+        <v>411755</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L36" s="5">
+        <f t="shared" ref="L36:S36" si="1">MIN(B28, L28)</f>
+        <v>6447</v>
+      </c>
+      <c r="M36" s="6">
+        <f t="shared" si="1"/>
+        <v>14311</v>
+      </c>
+      <c r="N36" s="6">
+        <f t="shared" si="1"/>
+        <v>22671</v>
+      </c>
+      <c r="O36" s="6">
+        <f t="shared" si="1"/>
+        <v>31439</v>
+      </c>
+      <c r="P36" s="6">
+        <f t="shared" si="1"/>
+        <v>40343</v>
+      </c>
+      <c r="Q36" s="6">
+        <f t="shared" si="1"/>
+        <v>87703</v>
+      </c>
+      <c r="R36" s="6">
+        <f t="shared" si="1"/>
+        <v>406863</v>
+      </c>
+      <c r="S36" s="6">
+        <f t="shared" si="1"/>
+        <v>1110895</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="5">
+        <f>MIN(B6, L6)</f>
+        <v>6958</v>
+      </c>
+      <c r="C37" s="5">
+        <f>MIN(C6, M6)</f>
+        <v>5193</v>
+      </c>
+      <c r="D37" s="5">
+        <f>MIN(D6, N6)</f>
+        <v>10093</v>
+      </c>
+      <c r="E37" s="5">
+        <f>MIN(E6, O6)</f>
+        <v>16642</v>
+      </c>
+      <c r="F37" s="5">
+        <f>MIN(F6, P6)</f>
+        <v>25419</v>
+      </c>
+      <c r="G37" s="6">
+        <f>MIN(G6, Q6)</f>
+        <v>75405</v>
+      </c>
+      <c r="H37" s="6">
+        <f>MIN(H6, R6)</f>
+        <v>297608</v>
+      </c>
+      <c r="I37" s="6">
+        <f>MIN(I6, S6)</f>
+        <v>821360</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L37" s="5">
+        <f t="shared" ref="L37:S37" si="2">MIN(B29, L29)</f>
+        <v>6852</v>
+      </c>
+      <c r="M37" s="6">
+        <f t="shared" si="2"/>
+        <v>15321</v>
+      </c>
+      <c r="N37" s="6">
+        <f t="shared" si="2"/>
+        <v>24372</v>
+      </c>
+      <c r="O37" s="6">
+        <f>MIN(E29, O29)</f>
+        <v>33860</v>
+      </c>
+      <c r="P37" s="6">
+        <f t="shared" si="2"/>
+        <v>43378</v>
+      </c>
+      <c r="Q37" s="6">
+        <f t="shared" si="2"/>
+        <v>94759</v>
+      </c>
+      <c r="R37" s="6">
+        <f t="shared" si="2"/>
+        <v>443086</v>
+      </c>
+      <c r="S37" s="6">
+        <f t="shared" si="2"/>
+        <v>1218069</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="5">
+        <f>MIN(B7, L7)</f>
+        <v>1687</v>
+      </c>
+      <c r="C38" s="5">
+        <f>MIN(C7, M7)</f>
+        <v>4910</v>
+      </c>
+      <c r="D38" s="5">
+        <f>MIN(D7, N7)</f>
         <v>10000</v>
       </c>
-    </row>
-    <row r="28" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F28" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G28" s="5">
-        <f t="shared" ref="G28:N31" si="0">MIN(B4, L4)</f>
-        <v>2013</v>
-      </c>
-      <c r="H28" s="5">
-        <f t="shared" si="0"/>
-        <v>360</v>
-      </c>
-      <c r="I28" s="5">
-        <f t="shared" si="0"/>
-        <v>458</v>
-      </c>
-      <c r="J28" s="5">
-        <f t="shared" si="0"/>
-        <v>614</v>
-      </c>
-      <c r="K28" s="5">
-        <f t="shared" si="0"/>
-        <v>731</v>
-      </c>
-      <c r="L28" s="5">
-        <f t="shared" si="0"/>
-        <v>1409</v>
-      </c>
-      <c r="M28" s="5">
-        <f t="shared" si="0"/>
-        <v>5563</v>
-      </c>
-      <c r="N28" s="5">
-        <f t="shared" si="0"/>
-        <v>15603</v>
-      </c>
-    </row>
-    <row r="29" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F29" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G29" s="6">
-        <f t="shared" si="0"/>
-        <v>5544</v>
-      </c>
-      <c r="H29" s="5">
-        <f t="shared" si="0"/>
-        <v>7631</v>
-      </c>
-      <c r="I29" s="5">
-        <f t="shared" si="0"/>
-        <v>16964</v>
-      </c>
-      <c r="J29" s="6">
-        <f t="shared" si="0"/>
-        <v>23254</v>
-      </c>
-      <c r="K29" s="6">
-        <f t="shared" si="0"/>
-        <v>29939</v>
-      </c>
-      <c r="L29" s="6">
-        <f t="shared" si="0"/>
-        <v>76049</v>
-      </c>
-      <c r="M29" s="6">
-        <f t="shared" si="0"/>
-        <v>147002</v>
-      </c>
-      <c r="N29" s="6">
-        <f t="shared" si="0"/>
-        <v>411755</v>
-      </c>
-    </row>
-    <row r="30" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F30" s="1" t="s">
+      <c r="E38" s="5">
+        <f>MIN(E7, O7)</f>
+        <v>16569</v>
+      </c>
+      <c r="F38" s="5">
+        <f>MIN(F7, P7)</f>
+        <v>26619</v>
+      </c>
+      <c r="G38" s="6">
+        <f>MIN(G7, Q7)</f>
+        <v>65404</v>
+      </c>
+      <c r="H38" s="6">
+        <f>MIN(H7, R7)</f>
+        <v>312154</v>
+      </c>
+      <c r="I38" s="6">
+        <f>MIN(I7, S7)</f>
+        <v>927490</v>
+      </c>
+      <c r="K38" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G30" s="5">
-        <f t="shared" si="0"/>
-        <v>6958</v>
-      </c>
-      <c r="H30" s="5">
-        <f t="shared" si="0"/>
-        <v>5193</v>
-      </c>
-      <c r="I30" s="5">
-        <f t="shared" si="0"/>
-        <v>10093</v>
-      </c>
-      <c r="J30" s="5">
-        <f t="shared" si="0"/>
-        <v>16642</v>
-      </c>
-      <c r="K30" s="5">
-        <f t="shared" si="0"/>
-        <v>25419</v>
-      </c>
-      <c r="L30" s="6">
-        <f t="shared" si="0"/>
-        <v>75405</v>
-      </c>
-      <c r="M30" s="6">
-        <f t="shared" si="0"/>
-        <v>297608</v>
-      </c>
-      <c r="N30" s="6">
-        <f t="shared" si="0"/>
-        <v>821360</v>
-      </c>
-    </row>
-    <row r="31" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G31" s="5">
-        <f t="shared" si="0"/>
-        <v>1687</v>
-      </c>
-      <c r="H31" s="5">
-        <f t="shared" si="0"/>
-        <v>4910</v>
-      </c>
-      <c r="I31" s="5">
-        <f t="shared" si="0"/>
-        <v>10000</v>
-      </c>
-      <c r="J31" s="5">
-        <f t="shared" si="0"/>
-        <v>16569</v>
-      </c>
-      <c r="K31" s="5">
-        <f t="shared" si="0"/>
-        <v>26619</v>
-      </c>
-      <c r="L31" s="6">
-        <f t="shared" si="0"/>
-        <v>65404</v>
-      </c>
-      <c r="M31" s="6">
-        <f t="shared" si="0"/>
-        <v>312154</v>
-      </c>
-      <c r="N31" s="6">
-        <f t="shared" si="0"/>
-        <v>927490</v>
+      <c r="L38" s="5">
+        <f t="shared" ref="L38:S38" si="3">MIN(B30, L30)</f>
+        <v>6853</v>
+      </c>
+      <c r="M38" s="6">
+        <f t="shared" si="3"/>
+        <v>15320</v>
+      </c>
+      <c r="N38" s="6">
+        <f t="shared" si="3"/>
+        <v>24370</v>
+      </c>
+      <c r="O38" s="6">
+        <f t="shared" si="3"/>
+        <v>33856</v>
+      </c>
+      <c r="P38" s="6">
+        <f t="shared" si="3"/>
+        <v>43365</v>
+      </c>
+      <c r="Q38" s="6">
+        <f t="shared" si="3"/>
+        <v>94764</v>
+      </c>
+      <c r="R38" s="6">
+        <f t="shared" si="3"/>
+        <v>443075</v>
+      </c>
+      <c r="S38" s="6">
+        <f t="shared" si="3"/>
+        <v>1218092</v>
       </c>
     </row>
   </sheetData>

</xml_diff>